<commit_message>
Herblore calculator from herbiboar
</commit_message>
<xml_diff>
--- a/Herbiboar.xlsx
+++ b/Herbiboar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Desktop\Misc_Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Desktop\Misc_Projects\Herbiboar_Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8BEDAB-3540-48C1-875A-40CB83134BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199F64E9-9416-494A-A0FC-DF8E7700DBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D7214999-E86C-49C0-A2ED-DC3DC39C4455}"/>
   </bookViews>
@@ -40,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="84">
   <si>
     <t>Guam</t>
   </si>
@@ -214,18 +236,6 @@
     <t>Cleaning Herbs XP</t>
   </si>
   <si>
-    <t>Super Combat</t>
-  </si>
-  <si>
-    <t>Super Strength</t>
-  </si>
-  <si>
-    <t>Super Restore</t>
-  </si>
-  <si>
-    <t>Super Defence</t>
-  </si>
-  <si>
     <t>POSSIBLE POTIONS</t>
   </si>
   <si>
@@ -256,9 +266,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Total Herblore XP Gained By End Of The Grind</t>
-  </si>
-  <si>
     <t>Potion XP (per potion)</t>
   </si>
   <si>
@@ -296,13 +303,25 @@
   </si>
   <si>
     <t>COMING SOON</t>
+  </si>
+  <si>
+    <t>Ranarr</t>
+  </si>
+  <si>
+    <t>Snapdrag.</t>
+  </si>
+  <si>
+    <t>HERBLORE SECONDARIES REQUIRED</t>
+  </si>
+  <si>
+    <t>Total Herblore XP Gained By End Of The Grind (assume 50xp/Herbi)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +356,14 @@
       <b/>
       <u/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -393,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -500,12 +527,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -515,21 +551,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -540,11 +564,38 @@
     <xf numFmtId="4" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,14 +609,11 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -585,35 +633,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -933,133 +992,132 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="5" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.21875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="5" customWidth="1"/>
     <col min="6" max="6" width="12.21875" style="5" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" style="5" customWidth="1"/>
     <col min="8" max="9" width="14.88671875" style="5" customWidth="1"/>
     <col min="10" max="10" width="3.6640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="43.33203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="4.44140625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="5" customWidth="1"/>
     <col min="14" max="14" width="10.21875" style="5" customWidth="1"/>
     <col min="15" max="15" width="3.21875" style="5" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="5" customWidth="1"/>
     <col min="17" max="17" width="9.5546875" style="5" customWidth="1"/>
     <col min="18" max="18" width="3.6640625" style="5" customWidth="1"/>
-    <col min="19" max="25" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="4.88671875" style="5" hidden="1" customWidth="1"/>
-    <col min="27" max="28" width="8.88671875" style="5" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="19" max="25" width="8.88671875" style="5" customWidth="1"/>
+    <col min="26" max="26" width="4.88671875" style="5" customWidth="1"/>
+    <col min="27" max="29" width="8.88671875" style="5" customWidth="1"/>
     <col min="30" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="59.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="24" t="s">
+    <row r="1" spans="1:28" ht="63.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="19"/>
+      <c r="B1" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="41" t="s">
+      <c r="G1" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="M1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="S1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="S1" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
       <c r="AA1"/>
       <c r="AB1"/>
     </row>
-    <row r="2" spans="1:28" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38">
+    <row r="2" spans="1:28" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17">
         <f>HLOOKUP(A2, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0.26400000000000001</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="37">
+      <c r="C2" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="16">
         <f>VLOOKUP(C2,Potion_Exp!A1:P44,3,FALSE)</f>
-        <v>25</v>
-      </c>
-      <c r="E2" s="37">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16">
         <f>3*B2</f>
         <v>0.79200000000000004</v>
       </c>
-      <c r="F2" s="39">
+      <c r="F2" s="18">
         <f>Q9*E2*D2</f>
-        <v>20908.800000000003</v>
-      </c>
-      <c r="G2" s="37">
-        <v>0</v>
-      </c>
-      <c r="H2" s="37">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16">
         <v>42</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="18">
         <f>((G2+H2)*D2)+(G2*Potion_Exp!C2)</f>
-        <v>1050</v>
-      </c>
-      <c r="K2" s="15">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
         <f>(50*Q9)+(M16)+M13</f>
-        <v>513217.76159999997</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="N2" s="46">
+        <v>52800</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="24">
         <v>3872597</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q2" s="31">
+      <c r="O2" s="7"/>
+      <c r="P2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="13">
         <v>87</v>
       </c>
       <c r="S2" s="1" t="s">
@@ -1070,7 +1128,7 @@
         <v>Attack</v>
       </c>
       <c r="U2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="V2"/>
       <c r="W2"/>
@@ -1084,43 +1142,43 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="21">
         <f>HLOOKUP(A3, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="42">
+      <c r="C3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="20">
         <f>VLOOKUP(C3,Potion_Exp!A1:P45,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="20">
         <f t="shared" ref="E3:E15" si="0">3*B3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="22">
         <f>Q9*E3*D3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
+      <c r="G3" s="20">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
         <v>383</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="22">
         <f>((G3+H3)*D3)+(G3*Potion_Exp!D2)</f>
         <v>0</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
       <c r="S3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1129,7 +1187,7 @@
         <v>Antipoison</v>
       </c>
       <c r="U3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="V3"/>
       <c r="W3"/>
@@ -1143,49 +1201,49 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="17">
         <f>HLOOKUP(A4, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="37">
+      <c r="C4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="16">
         <f>VLOOKUP(C4,Potion_Exp!A1:P44,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4" s="39">
+      <c r="F4" s="18">
         <f>Q9*E4*D4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="37">
-        <v>0</v>
-      </c>
-      <c r="H4" s="37">
+      <c r="G4" s="16">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16">
         <f>132+1433</f>
         <v>1565</v>
       </c>
-      <c r="I4" s="39">
+      <c r="I4" s="18">
         <f>((G4+H4)*D4)+(G4*Potion_Exp!E2)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="M4" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="29">
+      <c r="K4" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="39">
         <v>90</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -1200,7 +1258,7 @@
         <v>Serum 207</v>
       </c>
       <c r="V4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W4"/>
       <c r="X4"/>
@@ -1213,44 +1271,44 @@
       </c>
     </row>
     <row r="5" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="21">
         <f>HLOOKUP(A5, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="42">
+      <c r="C5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="20">
         <f>VLOOKUP(C5,Potion_Exp!A1:P44,6,FALSE)</f>
-        <v>67.5</v>
-      </c>
-      <c r="E5" s="42">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="22">
         <f>Q9*E5*D5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="42">
-        <v>0</v>
-      </c>
-      <c r="H5" s="42">
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
         <v>123</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="22">
         <f>((G5+H5)*D5)+(G5*Potion_Exp!F2)</f>
-        <v>8302.5</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="30"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="43"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="40"/>
       <c r="S5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1279,7 +1337,7 @@
         <v>Combat</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AA5">
         <v>35</v>
@@ -1289,44 +1347,44 @@
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="17">
         <f>HLOOKUP(A6, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>6.6400000000000001E-2</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="37">
+      <c r="C6" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="16">
         <f>VLOOKUP(C6,Potion_Exp!A1:P44,7,FALSE)</f>
-        <v>87.5</v>
-      </c>
-      <c r="E6" s="37">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>0.19919999999999999</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="18">
         <f>Q9*E6*D6</f>
-        <v>18406.079999999998</v>
-      </c>
-      <c r="G6" s="37">
-        <v>0</v>
-      </c>
-      <c r="H6" s="37">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="16">
         <v>87</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="18">
         <f>((G6+H6)*D6)+(G6*Potion_Exp!G2)</f>
-        <v>7612.5</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="43"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
       <c r="S6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1397,7 @@
         <v>Prayer</v>
       </c>
       <c r="V6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W6"/>
       <c r="X6"/>
@@ -1351,54 +1409,54 @@
         <v>24815</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="31.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:28" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="21">
         <f>HLOOKUP(A7, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="42">
+      <c r="C7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20">
         <f>VLOOKUP(C7,Potion_Exp!A1:P44,8,FALSE)</f>
-        <v>180</v>
-      </c>
-      <c r="E7" s="42">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="22">
         <f>Q9*E7*D7</f>
         <v>0</v>
       </c>
-      <c r="G7" s="42">
-        <v>0</v>
-      </c>
-      <c r="H7" s="42">
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20">
         <v>8</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="22">
         <f>((G7+H7)*D7)+(G7*Potion_Exp!H2)</f>
-        <v>1440</v>
-      </c>
-      <c r="K7" s="23">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12">
         <f>N2+K2</f>
-        <v>4385814.7615999999</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="N7" s="45">
+        <v>3925397</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="23">
         <v>2090743</v>
       </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q7" s="31">
+      <c r="O7" s="7"/>
+      <c r="P7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="13">
         <v>80</v>
       </c>
       <c r="S7" s="1" t="s">
@@ -1417,7 +1475,7 @@
         <v>Sara Brew</v>
       </c>
       <c r="W7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X7"/>
       <c r="Y7"/>
@@ -1428,44 +1486,44 @@
         <v>27473</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="17">
         <f>HLOOKUP(A8, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>8.9900000000000008E-2</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="37">
+      <c r="C8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="16">
         <f>VLOOKUP(C8,Potion_Exp!A1:P44,9,FALSE)</f>
-        <v>100</v>
-      </c>
-      <c r="E8" s="37">
+        <v>0</v>
+      </c>
+      <c r="E8" s="16">
         <f t="shared" si="0"/>
         <v>0.26970000000000005</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="18">
         <f>Q9*E8*D8</f>
-        <v>28480.320000000007</v>
-      </c>
-      <c r="G8" s="37">
-        <v>0</v>
-      </c>
-      <c r="H8" s="37">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
         <v>123</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="18">
         <f>((G8+H8)*D8)+(G8*Potion_Exp!I2)</f>
-        <v>12300</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
       <c r="S8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1486,7 +1544,7 @@
         <v>Antivenom</v>
       </c>
       <c r="X8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Y8"/>
       <c r="AA8">
@@ -1497,49 +1555,49 @@
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="21">
         <f>HLOOKUP(A9, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>9.6799999999999997E-2</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="42">
+      <c r="C9" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="20">
         <f>VLOOKUP(C9,Potion_Exp!A1:P44,10,FALSE)</f>
-        <v>194</v>
-      </c>
-      <c r="E9" s="42">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
         <f t="shared" si="0"/>
         <v>0.29039999999999999</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="22">
         <f>Q9*E9*D9</f>
-        <v>59492.505599999997</v>
-      </c>
-      <c r="G9" s="42">
-        <v>0</v>
-      </c>
-      <c r="H9" s="42">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
         <v>120</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="22">
         <f>((G9+H9)*D9)+(G9*Potion_Exp!J2)</f>
-        <v>23280</v>
-      </c>
-      <c r="K9" s="16" t="str">
+        <v>0</v>
+      </c>
+      <c r="K9" s="27" t="str">
         <f>IF((K7-M19)&lt;0,"THIS IS NOT ENOUGH. YOU STILL NEED THIS XP:","THIS IS ENOUGH. YOU HAVE EXTRA HERBLORE XP OF:")</f>
-        <v>THIS IS ENOUGH. YOU HAVE EXTRA HERBLORE XP OF:</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="31">
+        <v>THIS IS NOT ENOUGH. YOU STILL NEED THIS XP:</v>
+      </c>
+      <c r="M9" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="13">
         <v>1056</v>
       </c>
       <c r="S9" s="1" t="s">
@@ -1562,7 +1620,7 @@
         <v>Stamina</v>
       </c>
       <c r="X9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Y9"/>
       <c r="AA9">
@@ -1573,39 +1631,39 @@
       </c>
     </row>
     <row r="10" spans="1:28" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="17">
         <f>HLOOKUP(A10, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0.12050000000000001</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="37">
+      <c r="C10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="16">
         <f>VLOOKUP(C10,Potion_Exp!A1:P44,11,FALSE)</f>
-        <v>125</v>
-      </c>
-      <c r="E10" s="37">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16">
         <f t="shared" si="0"/>
         <v>0.36150000000000004</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="18">
         <f>Q9*E10*D10</f>
-        <v>47718</v>
-      </c>
-      <c r="G10" s="37">
-        <v>0</v>
-      </c>
-      <c r="H10" s="37">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
         <v>75</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="18">
         <f>((G10+H10)*D10)+(G10*Potion_Exp!K2)</f>
-        <v>9375</v>
-      </c>
-      <c r="K10" s="16"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="27"/>
       <c r="S10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1618,7 +1676,7 @@
         <v>Weapon poison</v>
       </c>
       <c r="V10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W10"/>
       <c r="X10"/>
@@ -1630,42 +1688,42 @@
         <v>37224</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
+    <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="21">
         <f>HLOOKUP(A11, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>3.85E-2</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="42">
+      <c r="C11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="20">
         <f>VLOOKUP(C11,Potion_Exp!A1:P44,12,FALSE)</f>
-        <v>142.5</v>
-      </c>
-      <c r="E11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20">
         <f t="shared" si="0"/>
         <v>0.11549999999999999</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="22">
         <f>Q9*E11*D11</f>
-        <v>17380.439999999999</v>
-      </c>
-      <c r="G11" s="42">
-        <v>0</v>
-      </c>
-      <c r="H11" s="42">
+        <v>0</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20">
         <v>21</v>
       </c>
-      <c r="I11" s="44">
+      <c r="I11" s="22">
         <f>((G11+H11)*D11)+(G11*Potion_Exp!L2)</f>
-        <v>2992.5</v>
-      </c>
-      <c r="K11" s="23">
+        <v>0</v>
+      </c>
+      <c r="K11" s="12">
         <f>ABS(K7-M19)</f>
-        <v>38.761599999852479</v>
+        <v>460379</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>8</v>
@@ -1679,7 +1737,7 @@
         <v>Sanfew serum</v>
       </c>
       <c r="V11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W11"/>
       <c r="X11"/>
@@ -1691,46 +1749,46 @@
         <v>41171</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="17">
         <f>HLOOKUP(A12, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0.1153</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="37">
+      <c r="C12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="16">
         <f>VLOOKUP(C12,Potion_Exp!A1:P44,13,FALSE)</f>
-        <v>150</v>
-      </c>
-      <c r="E12" s="37">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16">
         <f t="shared" si="0"/>
         <v>0.34589999999999999</v>
       </c>
-      <c r="F12" s="39">
+      <c r="F12" s="18">
         <f>Q9*E12*D12</f>
-        <v>54790.559999999998</v>
-      </c>
-      <c r="G12" s="37">
-        <v>0</v>
-      </c>
-      <c r="H12" s="37">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
         <v>90</v>
       </c>
-      <c r="I12" s="39">
+      <c r="I12" s="18">
         <f>((G12+H12)*D12)+(G12*Potion_Exp!M2)</f>
-        <v>13500</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="20"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="31"/>
       <c r="S12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1747,7 +1805,7 @@
         <v>Battlemage</v>
       </c>
       <c r="W12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X12"/>
       <c r="Y12"/>
@@ -1759,49 +1817,49 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="21">
         <f>HLOOKUP(A13, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>0.1016</v>
       </c>
-      <c r="C13" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="42">
+      <c r="C13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="20">
         <f>VLOOKUP(C13,Potion_Exp!A1:P44,14,FALSE)</f>
-        <v>157.5</v>
-      </c>
-      <c r="E13" s="42">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
         <f t="shared" si="0"/>
         <v>0.30479999999999996</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="22">
         <f>Q9*E13*D13</f>
-        <v>50694.335999999996</v>
-      </c>
-      <c r="G13" s="42">
-        <v>0</v>
-      </c>
-      <c r="H13" s="42">
+        <v>0</v>
+      </c>
+      <c r="G13" s="20">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
         <v>81</v>
       </c>
-      <c r="I13" s="44">
+      <c r="I13" s="22">
         <f>((G13+H13)*D13)+(G13*Potion_Exp!N2)</f>
-        <v>12757.5</v>
-      </c>
-      <c r="K13" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13" s="21">
+        <v>0</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="32">
         <f>SUM(F2:F15)</f>
-        <v>351457.76159999997</v>
-      </c>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="34"/>
       <c r="S13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1826,7 +1884,7 @@
         <v>None</v>
       </c>
       <c r="Y13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AA13">
         <v>43</v>
@@ -1836,39 +1894,39 @@
       </c>
     </row>
     <row r="14" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="38">
+      <c r="B14" s="17">
         <f>HLOOKUP(A14, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="37">
+      <c r="C14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="16">
         <f>VLOOKUP(C14,Potion_Exp!A1:P44,15,FALSE)</f>
-        <v>162.5</v>
-      </c>
-      <c r="E14" s="37">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
         <f t="shared" si="0"/>
         <v>0.2112</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="18">
         <f>Q9*E14*D14</f>
-        <v>36241.919999999998</v>
-      </c>
-      <c r="G14" s="37">
-        <v>0</v>
-      </c>
-      <c r="H14" s="37">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
         <v>96</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="18">
         <f>((G14+H14)*D14)+(G14*Potion_Exp!O2)</f>
-        <v>15600</v>
-      </c>
-      <c r="K14" s="34"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="28"/>
       <c r="S14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1885,7 +1943,7 @@
         <v>Ancient Brew</v>
       </c>
       <c r="W14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X14"/>
       <c r="Y14"/>
@@ -1896,49 +1954,49 @@
         <v>55649</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+    <row r="15" spans="1:28" ht="21" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="21">
         <f>HLOOKUP(A15, Herb_Rates!A1:P70, (Q2-29),FALSE)/100</f>
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="42">
+      <c r="C15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="20">
         <f>VLOOKUP(C15,Potion_Exp!A1:P44,16,FALSE)</f>
-        <v>150</v>
-      </c>
-      <c r="E15" s="42">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20">
         <f t="shared" si="0"/>
         <v>0.10949999999999999</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="22">
         <f>Q9*E15*D15</f>
-        <v>17344.8</v>
-      </c>
-      <c r="G15" s="42">
-        <v>0</v>
-      </c>
-      <c r="H15" s="42">
+        <v>0</v>
+      </c>
+      <c r="G15" s="20">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
         <v>5</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="22">
         <f>((G15+H15)*D15)+(G15*Potion_Exp!P2)</f>
-        <v>750</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
       <c r="S15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1955,7 +2013,7 @@
         <v>None</v>
       </c>
       <c r="W15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="X15"/>
       <c r="Y15"/>
@@ -1967,14 +2025,14 @@
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="M16" s="22">
+      <c r="M16" s="26">
         <f>SUM(I2:I15)</f>
-        <v>108960</v>
-      </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
       <c r="S16"/>
       <c r="T16"/>
       <c r="U16"/>
@@ -1989,7 +2047,18 @@
         <v>67983</v>
       </c>
     </row>
-    <row r="17" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
       <c r="S17"/>
       <c r="T17"/>
       <c r="U17"/>
@@ -2004,14 +2073,47 @@
         <v>75127</v>
       </c>
     </row>
-    <row r="18" spans="13:28" x14ac:dyDescent="0.3">
-      <c r="M18" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+    <row r="18" spans="1:28" ht="32.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="51" t="str" cm="1">
+        <f t="array" ref="B18">_xlfn.IFS(C2="None","n/a",C2="Attack","Eye of Newt")</f>
+        <v>n/a</v>
+      </c>
+      <c r="C18" s="49">
+        <f>IF(C2="None",0,E2*Q9+H2)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="51" t="str" cm="1">
+        <f t="array" ref="E18">_xlfn.IFS(C7=W7,"n/a",C7=T7,"Toad Legs",C7=U7,"Yew Roots",C7=V7,"Crushed Bird Nests")</f>
+        <v>n/a</v>
+      </c>
+      <c r="F18" s="49">
+        <f>IF(C7="None",0,E7*Q9+H7)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="51" t="str" cm="1">
+        <f t="array" ref="H18">_xlfn.IFS(C12=W12,"n/a",C12=T12,"White Berries",C12=U12,"Blood+Zammy Wine",C12=V12,"Blood+Potato Cactus")</f>
+        <v>n/a</v>
+      </c>
+      <c r="I18" s="50">
+        <f>IF(C12="None",0,E12*Q9+H12)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
       <c r="S18"/>
       <c r="T18"/>
       <c r="U18"/>
@@ -2026,15 +2128,48 @@
         <v>83014</v>
       </c>
     </row>
-    <row r="19" spans="13:28" x14ac:dyDescent="0.3">
-      <c r="M19" s="22">
+    <row r="19" spans="1:28" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="51" t="str" cm="1">
+        <f t="array" ref="B19">_xlfn.IFS(C3="None","n/a",C3="Antipoison","Unicorn Horn Dust")</f>
+        <v>n/a</v>
+      </c>
+      <c r="C19" s="49">
+        <f>IF(C3="None",0,E3*Q9+H3)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="51" t="str" cm="1">
+        <f t="array" ref="E19">_xlfn.IFS(C8=X8,"n/a",C8=T8,"Eye of Newt",C8=U8,"Unicorn Horn Dust",C8=V8,"Magic Roots",C8=W8,"Zulrah Scales (x20)")</f>
+        <v>n/a</v>
+      </c>
+      <c r="F19" s="49">
+        <f>IF(C8="None",0,E8*Q9+H8)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="51" t="str" cm="1">
+        <f t="array" ref="H19">_xlfn.IFS(C13=Y13,"n/a",C13=T13,"Dragon Scale Dust",C13=U13,"Potato Cacti",C13=V13,"Lava scale shards",C13=W13,"Vork Bone Dust",C13=X13,"Lava scale shards")</f>
+        <v>n/a</v>
+      </c>
+      <c r="I19" s="50">
+        <f>IF(C13="None",0,E13*Q9+H13)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="26">
         <f>VLOOKUP(Q2+1,AA2:AB69,2)</f>
         <v>4385776</v>
       </c>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
       <c r="S19"/>
       <c r="T19"/>
       <c r="U19"/>
@@ -2049,7 +2184,48 @@
         <v>91721</v>
       </c>
     </row>
-    <row r="20" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="32.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="51" t="str" cm="1">
+        <f t="array" ref="B20">_xlfn.IFS(C4="None","n/a",C4="Strength","Limpwurt Root",C4="Serum 207", "Ashes")</f>
+        <v>n/a</v>
+      </c>
+      <c r="C20" s="49">
+        <f>IF(C4="None",0,E4*Q9+H4)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="51" t="str" cm="1">
+        <f t="array" ref="E20">_xlfn.IFS(C9=X9,"n/a",C9=T9,"Snape Grass",C9=U9,"Mort Myre Fungi",C9=V9,"Kebbit Teeth",C9=W9,"Amaylase Crystals (x4)")</f>
+        <v>n/a</v>
+      </c>
+      <c r="F20" s="49">
+        <f>IF(C9="None",0,E9*Q9+H9)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="51" t="str" cm="1">
+        <f t="array" ref="H20">_xlfn.IFS(C14=W14,"n/a",C14=T14,"Lily of Sands",C14=U14,"Zammy Wine",C14=V14,"Nihil Dust")</f>
+        <v>n/a</v>
+      </c>
+      <c r="I20" s="50">
+        <f>IF(C14="None",0,E14*Q9+H14)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="46"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
       <c r="AA20" s="5">
         <v>50</v>
       </c>
@@ -2057,7 +2233,41 @@
         <v>101333</v>
       </c>
     </row>
-    <row r="21" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" ht="32.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="51" t="str" cm="1">
+        <f t="array" ref="B21">_xlfn.IFS(C5=Z5,"n/a",C5=T5,"2 guam, 1 marrentil, tea cup",C5=U5,"Volcanic Ash",C5=V5,"Red Spider Eggs",C5=W5,"Silver Dust + Garlic",C5="Energy","Chocolate Dust",C5=Y5,"Goat Horn Dust")</f>
+        <v>n/a</v>
+      </c>
+      <c r="C21" s="49">
+        <f>IF(C5="None",0,E5*Q9+H5)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="51" t="str" cm="1">
+        <f t="array" ref="E21">_xlfn.IFS(C10=V10,"n/a",C10=T10,"Limpwurt Root",C10=U10,"Red Spider Eggs")</f>
+        <v>n/a</v>
+      </c>
+      <c r="F21" s="49">
+        <f>IF(C10="None",0,E10*Q9+H10)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="51" t="str" cm="1">
+        <f t="array" ref="H21">_xlfn.IFS(C15=W15,"n/a",C15=T15,"Zammy Wine",C15=U15,"Super Set",C15=V15,"Anti-venom")</f>
+        <v>n/a</v>
+      </c>
+      <c r="I21" s="50">
+        <f>IF(C15="None",0,E15*Q9+H15)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="45"/>
       <c r="AA21" s="5">
         <v>51</v>
       </c>
@@ -2065,7 +2275,32 @@
         <v>111945</v>
       </c>
     </row>
-    <row r="22" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="51" t="str" cm="1">
+        <f t="array" ref="B22">_xlfn.IFS(C6=V6,"n/a",C6=T6,"White Berries",C6=U6,"Snape Grass")</f>
+        <v>n/a</v>
+      </c>
+      <c r="C22" s="49">
+        <f>IF(C6="None",0,E6*Q9+H6)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="51" t="str" cm="1">
+        <f t="array" ref="E22">_xlfn.IFS(C11=V11,"n/a",C11=T11,"Red Spider Eggs",C11=U11,"3 ingredients (check wiki)")</f>
+        <v>n/a</v>
+      </c>
+      <c r="F22" s="49">
+        <f>IF(C11="None",0,E11*Q9+H11)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="47"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="48"/>
       <c r="AA22" s="5">
         <v>52</v>
       </c>
@@ -2073,7 +2308,7 @@
         <v>123660</v>
       </c>
     </row>
-    <row r="23" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA23" s="5">
         <v>53</v>
       </c>
@@ -2081,7 +2316,7 @@
         <v>136594</v>
       </c>
     </row>
-    <row r="24" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA24" s="5">
         <v>54</v>
       </c>
@@ -2089,7 +2324,7 @@
         <v>150872</v>
       </c>
     </row>
-    <row r="25" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA25" s="5">
         <v>55</v>
       </c>
@@ -2097,7 +2332,7 @@
         <v>166636</v>
       </c>
     </row>
-    <row r="26" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA26" s="5">
         <v>56</v>
       </c>
@@ -2105,7 +2340,7 @@
         <v>184040</v>
       </c>
     </row>
-    <row r="27" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA27" s="5">
         <v>57</v>
       </c>
@@ -2113,7 +2348,7 @@
         <v>203254</v>
       </c>
     </row>
-    <row r="28" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA28" s="5">
         <v>58</v>
       </c>
@@ -2121,7 +2356,7 @@
         <v>224466</v>
       </c>
     </row>
-    <row r="29" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA29" s="5">
         <v>59</v>
       </c>
@@ -2129,7 +2364,7 @@
         <v>247886</v>
       </c>
     </row>
-    <row r="30" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA30" s="5">
         <v>60</v>
       </c>
@@ -2137,7 +2372,7 @@
         <v>273742</v>
       </c>
     </row>
-    <row r="31" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA31" s="5">
         <v>61</v>
       </c>
@@ -2145,7 +2380,7 @@
         <v>302288</v>
       </c>
     </row>
-    <row r="32" spans="13:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="AA32" s="5">
         <v>62</v>
       </c>
@@ -2450,21 +2685,22 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="A17:I17"/>
     <mergeCell ref="M18:Q18"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="M1:Q1"/>
     <mergeCell ref="M4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="M9:P9"/>
     <mergeCell ref="K4:K6"/>
     <mergeCell ref="M16:Q16"/>
     <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="M13:Q13"/>
   </mergeCells>
   <dataValidations count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0D1F95E5-03DF-4A88-8434-682604B856F5}">
@@ -2501,7 +2737,7 @@
       <formula1>$T$12:$W$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{FF6170B1-045D-47EB-82F4-4CEC5D01C595}">
-      <formula1>$T$13:$Z$13</formula1>
+      <formula1>$T$13:$Y$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{B4E1E3E2-1BC2-48E5-AB76-D9D6805C2065}">
       <formula1>$T$14:$W$14</formula1>
@@ -2511,6 +2747,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5937,7 +6174,7 @@
         <v>6.48</v>
       </c>
       <c r="P67">
-        <f t="shared" ref="P67:P100" si="1">SUM(B67:O67)</f>
+        <f t="shared" ref="P67:P70" si="1">SUM(B67:O67)</f>
         <v>100</v>
       </c>
     </row>
@@ -6781,7 +7018,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
@@ -6950,7 +7187,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -6998,7 +7235,7 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>44</v>
       </c>
@@ -7022,7 +7259,7 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>45</v>
       </c>
@@ -7095,7 +7332,7 @@
       </c>
       <c r="P38" s="4"/>
     </row>
-    <row r="39" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>48</v>
       </c>
@@ -7169,7 +7406,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>51</v>
       </c>
@@ -7221,7 +7458,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="2">

</xml_diff>